<commit_message>
fixed excel and view bugs
</commit_message>
<xml_diff>
--- a/Mélodie/Book1.xlsx
+++ b/Mélodie/Book1.xlsx
@@ -26,7 +26,7 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
   <si>
-    <t>kearnejb@uwec.edu</t>
+    <t>stupkajr@uwec.edu</t>
   </si>
 </sst>
 </file>
@@ -358,7 +358,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>